<commit_message>
adds border for each angajat
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/templates/StatSalarii.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/templates/StatSalarii.xlsx
@@ -390,8 +390,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,10 +407,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,8 +694,8 @@
   </sheetPr>
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -724,32 +724,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="L4" s="18" t="s">
         <v>1</v>
       </c>
@@ -757,11 +757,11 @@
       <c r="N4" s="18"/>
     </row>
     <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="L5" s="19" t="s">
         <v>67</v>
       </c>
@@ -929,14 +929,14 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
@@ -988,10 +988,10 @@
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1041,10 +1041,10 @@
       <c r="I13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="24"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="T21" s="15"/>
       <c r="U21" s="15"/>
     </row>
-    <row r="22" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1294,7 +1294,7 @@
       <c r="U22" s="15"/>
       <c r="V22" s="7"/>
     </row>
-    <row r="23" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1318,7 +1318,7 @@
       <c r="U23" s="15"/>
       <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1342,7 +1342,7 @@
       <c r="U24" s="15"/>
       <c r="V24" s="7"/>
     </row>
-    <row r="25" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1366,7 +1366,7 @@
       <c r="U25" s="15"/>
       <c r="V25" s="7"/>
     </row>
-    <row r="26" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1389,7 +1389,7 @@
       <c r="T26" s="15"/>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1412,7 +1412,7 @@
       <c r="T27" s="15"/>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1435,7 +1435,7 @@
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
     </row>
-    <row r="29" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1505,6 +1505,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="D11:E11"/>
@@ -1514,11 +1519,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
more completion on stat salarii
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/templates/StatSalarii.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/templates/StatSalarii.xlsx
@@ -364,59 +364,125 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,814 +768,815 @@
   </sheetPr>
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="L4" s="17" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="L4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-    </row>
-    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+    </row>
+    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="L5" s="18" t="s">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="L5" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="13">
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="29">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="34">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="34">
         <v>4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>7</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>8</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>9</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>10</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>11</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>12</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>13</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <v>14</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="1">
         <v>15</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="1">
         <v>16</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="1">
         <v>17</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="1">
         <v>18</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="1">
         <v>19</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="35"/>
+      <c r="F9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="9" t="s">
+      <c r="H9" s="26"/>
+      <c r="I9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="U9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="10">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8">
         <v>0.75</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8" t="s">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8" t="s">
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="U10" s="6"/>
+      <c r="U10" s="9"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="P11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="Q11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="8" t="s">
+      <c r="T11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="U11" s="6"/>
+      <c r="U11" s="9"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="16" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8" t="s">
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="9"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="21"/>
+      <c r="L13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="8" t="s">
+      <c r="Q13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="R13" s="8" t="s">
+      <c r="R13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="8" t="s">
+      <c r="T13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="U13" s="6"/>
+      <c r="U13" s="9"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="12">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="Q14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="13"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="12"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="7"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="16"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="7"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="16"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="7"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="16"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="7"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="16"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>